<commit_message>
New version of matmult experiment definition
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen_matmult_circle_pi4.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen_matmult_circle_pi4.xlsx
@@ -457,10 +457,10 @@
   <dimension ref="A1:AMJ74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.30859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -637,14 +637,14 @@
       </c>
       <c r="R3" s="13" t="n">
         <f aca="false">INT(T3/U3)</f>
-        <v>1300</v>
+        <v>1020</v>
       </c>
       <c r="S3" s="14" t="n">
-        <v>26008</v>
+        <v>20403</v>
       </c>
       <c r="T3" s="13" t="n">
         <f aca="false">INT(S3/10)</f>
-        <v>2600</v>
+        <v>2040</v>
       </c>
       <c r="U3" s="11" t="n">
         <v>2</v>
@@ -702,14 +702,14 @@
       </c>
       <c r="R4" s="13" t="n">
         <f aca="false">INT(T4/U4)</f>
-        <v>15768</v>
+        <v>15679</v>
       </c>
       <c r="S4" s="14" t="n">
-        <v>315372</v>
+        <v>313588</v>
       </c>
       <c r="T4" s="13" t="n">
         <f aca="false">INT(S4/10)</f>
-        <v>31537</v>
+        <v>31358</v>
       </c>
       <c r="U4" s="11" t="n">
         <v>2</v>
@@ -767,14 +767,14 @@
       </c>
       <c r="R5" s="13" t="n">
         <f aca="false">INT(T5/U5)</f>
-        <v>83797</v>
+        <v>83660</v>
       </c>
       <c r="S5" s="14" t="n">
-        <v>1675942</v>
+        <v>1673203</v>
       </c>
       <c r="T5" s="13" t="n">
         <f aca="false">INT(S5/10)</f>
-        <v>167594</v>
+        <v>167320</v>
       </c>
       <c r="U5" s="11" t="n">
         <v>2</v>
@@ -832,14 +832,14 @@
       </c>
       <c r="R6" s="13" t="n">
         <f aca="false">INT(T6/U6)</f>
-        <v>119211</v>
+        <v>119061</v>
       </c>
       <c r="S6" s="14" t="n">
-        <v>2384227</v>
+        <v>2381226</v>
       </c>
       <c r="T6" s="13" t="n">
         <f aca="false">INT(S6/10)</f>
-        <v>238422</v>
+        <v>238122</v>
       </c>
       <c r="U6" s="11" t="n">
         <v>2</v>
@@ -897,14 +897,14 @@
       </c>
       <c r="R7" s="13" t="n">
         <f aca="false">INT(T7/U7)</f>
-        <v>237347</v>
+        <v>237740</v>
       </c>
       <c r="S7" s="14" t="n">
-        <v>4746952</v>
+        <v>4754819</v>
       </c>
       <c r="T7" s="13" t="n">
         <f aca="false">INT(S7/10)</f>
-        <v>474695</v>
+        <v>475481</v>
       </c>
       <c r="U7" s="11" t="n">
         <v>2</v>
@@ -962,14 +962,14 @@
       </c>
       <c r="R8" s="13" t="n">
         <f aca="false">INT(T8/U8)</f>
-        <v>212649</v>
+        <v>212477</v>
       </c>
       <c r="S8" s="14" t="n">
-        <v>4252987</v>
+        <v>4249541</v>
       </c>
       <c r="T8" s="13" t="n">
         <f aca="false">INT(S8/10)</f>
-        <v>425298</v>
+        <v>424954</v>
       </c>
       <c r="U8" s="11" t="n">
         <v>2</v>
@@ -1027,14 +1027,14 @@
       </c>
       <c r="R9" s="13" t="n">
         <f aca="false">INT(T9/U9)</f>
-        <v>282925</v>
+        <v>282927</v>
       </c>
       <c r="S9" s="14" t="n">
-        <v>5658517</v>
+        <v>5658556</v>
       </c>
       <c r="T9" s="13" t="n">
         <f aca="false">INT(S9/10)</f>
-        <v>565851</v>
+        <v>565855</v>
       </c>
       <c r="U9" s="11" t="n">
         <v>2</v>
@@ -1092,14 +1092,14 @@
       </c>
       <c r="R10" s="13" t="n">
         <f aca="false">INT(T10/U10)</f>
-        <v>539676</v>
+        <v>538966</v>
       </c>
       <c r="S10" s="14" t="n">
-        <v>10793537</v>
+        <v>10779339</v>
       </c>
       <c r="T10" s="13" t="n">
         <f aca="false">INT(S10/10)</f>
-        <v>1079353</v>
+        <v>1077933</v>
       </c>
       <c r="U10" s="11" t="n">
         <v>2</v>
@@ -1149,7 +1149,7 @@
         <v>100</v>
       </c>
       <c r="O11" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P11" s="0" t="n">
         <v>0</v>
@@ -1159,15 +1159,15 @@
       </c>
       <c r="R11" s="16" t="n">
         <f aca="false">INT(T11/U11)</f>
-        <v>237347</v>
+        <v>237740</v>
       </c>
       <c r="S11" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4746952</v>
+        <v>4754819</v>
       </c>
       <c r="T11" s="16" t="n">
         <f aca="false">INT(S11/10)</f>
-        <v>474695</v>
+        <v>475481</v>
       </c>
       <c r="U11" s="0" t="n">
         <v>2</v>
@@ -1219,25 +1219,25 @@
         <v>100</v>
       </c>
       <c r="O12" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P12" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q12" s="0" t="n">
-        <v>131072</v>
+        <v>0</v>
       </c>
       <c r="R12" s="16" t="n">
         <f aca="false">INT(T12/U12)</f>
-        <v>237347</v>
+        <v>237740</v>
       </c>
       <c r="S12" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4746952</v>
+        <v>4754819</v>
       </c>
       <c r="T12" s="16" t="n">
         <f aca="false">INT(S12/10)</f>
-        <v>474695</v>
+        <v>475481</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>2</v>
@@ -1291,25 +1291,25 @@
         <v>20</v>
       </c>
       <c r="O13" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P13" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q13" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R13" s="16" t="n">
         <f aca="false">INT(T13/U13)</f>
-        <v>1300</v>
+        <v>1020</v>
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">S$3</f>
-        <v>26008</v>
+        <v>20403</v>
       </c>
       <c r="T13" s="16" t="n">
         <f aca="false">INT(S13/10)</f>
-        <v>2600</v>
+        <v>2040</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>2</v>
@@ -1363,25 +1363,25 @@
         <v>50</v>
       </c>
       <c r="O14" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P14" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q14" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R14" s="16" t="n">
         <f aca="false">INT(T14/U14)</f>
-        <v>15768</v>
+        <v>15679</v>
       </c>
       <c r="S14" s="0" t="n">
         <f aca="false">S$4</f>
-        <v>315372</v>
+        <v>313588</v>
       </c>
       <c r="T14" s="16" t="n">
         <f aca="false">INT(S14/10)</f>
-        <v>31537</v>
+        <v>31358</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>2</v>
@@ -1435,25 +1435,25 @@
         <v>80</v>
       </c>
       <c r="O15" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P15" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q15" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R15" s="16" t="n">
         <f aca="false">INT(T15/U15)</f>
-        <v>83797</v>
+        <v>83660</v>
       </c>
       <c r="S15" s="0" t="n">
         <f aca="false">S$5</f>
-        <v>1675942</v>
+        <v>1673203</v>
       </c>
       <c r="T15" s="16" t="n">
         <f aca="false">INT(S15/10)</f>
-        <v>167594</v>
+        <v>167320</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>2</v>
@@ -1507,25 +1507,25 @@
         <v>90</v>
       </c>
       <c r="O16" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P16" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q16" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R16" s="16" t="n">
         <f aca="false">INT(T16/U16)</f>
-        <v>119211</v>
+        <v>119061</v>
       </c>
       <c r="S16" s="0" t="n">
         <f aca="false">S$6</f>
-        <v>2384227</v>
+        <v>2381226</v>
       </c>
       <c r="T16" s="16" t="n">
         <f aca="false">INT(S16/10)</f>
-        <v>238422</v>
+        <v>238122</v>
       </c>
       <c r="U16" s="0" t="n">
         <v>2</v>
@@ -1579,25 +1579,25 @@
         <v>100</v>
       </c>
       <c r="O17" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P17" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q17" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R17" s="16" t="n">
         <f aca="false">INT(T17/U17)</f>
-        <v>237347</v>
+        <v>237740</v>
       </c>
       <c r="S17" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4746952</v>
+        <v>4754819</v>
       </c>
       <c r="T17" s="16" t="n">
         <f aca="false">INT(S17/10)</f>
-        <v>474695</v>
+        <v>475481</v>
       </c>
       <c r="U17" s="0" t="n">
         <v>2</v>
@@ -1651,25 +1651,25 @@
         <v>110</v>
       </c>
       <c r="O18" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P18" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q18" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R18" s="16" t="n">
         <f aca="false">INT(T18/U18)</f>
-        <v>212649</v>
+        <v>212477</v>
       </c>
       <c r="S18" s="0" t="n">
         <f aca="false">S$8</f>
-        <v>4252987</v>
+        <v>4249541</v>
       </c>
       <c r="T18" s="16" t="n">
         <f aca="false">INT(S18/10)</f>
-        <v>425298</v>
+        <v>424954</v>
       </c>
       <c r="U18" s="0" t="n">
         <v>2</v>
@@ -1725,25 +1725,25 @@
         <v>120</v>
       </c>
       <c r="O19" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P19" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q19" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R19" s="16" t="n">
         <f aca="false">INT(T19/U19)</f>
-        <v>282925</v>
+        <v>282927</v>
       </c>
       <c r="S19" s="0" t="n">
         <f aca="false">S$9</f>
-        <v>5658517</v>
+        <v>5658556</v>
       </c>
       <c r="T19" s="16" t="n">
         <f aca="false">INT(S19/10)</f>
-        <v>565851</v>
+        <v>565855</v>
       </c>
       <c r="U19" s="0" t="n">
         <v>2</v>
@@ -1799,25 +1799,25 @@
         <v>150</v>
       </c>
       <c r="O20" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="P20" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="Q20" s="0" t="n">
-        <v>131072</v>
+        <v>4096</v>
       </c>
       <c r="R20" s="16" t="n">
         <f aca="false">INT(T20/U20)</f>
-        <v>539676</v>
+        <v>538966</v>
       </c>
       <c r="S20" s="0" t="n">
         <f aca="false">S$10</f>
-        <v>10793537</v>
+        <v>10779339</v>
       </c>
       <c r="T20" s="16" t="n">
         <f aca="false">INT(S20/10)</f>
-        <v>1079353</v>
+        <v>1077933</v>
       </c>
       <c r="U20" s="0" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
New experiments and some fixes
</commit_message>
<xml_diff>
--- a/experiment/xlsx/experiments_Mälardalen_matmult_circle_pi4.xlsx
+++ b/experiment/xlsx/experiments_Mälardalen_matmult_circle_pi4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="55">
   <si>
     <t xml:space="preserve">xrtos or circle</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_WRITEATTACK1_INPUTSIZE150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BENCH_MÄLARDALEN_MATMULT_CORES4_MEMORYPROFILE_INPUTSIZE100</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
   <dimension ref="A1:AMJ74"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.31640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
@@ -637,14 +640,14 @@
       </c>
       <c r="R3" s="13" t="n">
         <f aca="false">INT(T3/U3)</f>
-        <v>1020</v>
+        <v>1325</v>
       </c>
       <c r="S3" s="14" t="n">
-        <v>20403</v>
+        <v>26512</v>
       </c>
       <c r="T3" s="13" t="n">
         <f aca="false">INT(S3/10)</f>
-        <v>2040</v>
+        <v>2651</v>
       </c>
       <c r="U3" s="11" t="n">
         <v>2</v>
@@ -702,14 +705,14 @@
       </c>
       <c r="R4" s="13" t="n">
         <f aca="false">INT(T4/U4)</f>
-        <v>15679</v>
+        <v>15690</v>
       </c>
       <c r="S4" s="14" t="n">
-        <v>313588</v>
+        <v>313813</v>
       </c>
       <c r="T4" s="13" t="n">
         <f aca="false">INT(S4/10)</f>
-        <v>31358</v>
+        <v>31381</v>
       </c>
       <c r="U4" s="11" t="n">
         <v>2</v>
@@ -767,14 +770,14 @@
       </c>
       <c r="R5" s="13" t="n">
         <f aca="false">INT(T5/U5)</f>
-        <v>83660</v>
+        <v>83701</v>
       </c>
       <c r="S5" s="14" t="n">
-        <v>1673203</v>
+        <v>1674035</v>
       </c>
       <c r="T5" s="13" t="n">
         <f aca="false">INT(S5/10)</f>
-        <v>167320</v>
+        <v>167403</v>
       </c>
       <c r="U5" s="11" t="n">
         <v>2</v>
@@ -832,14 +835,14 @@
       </c>
       <c r="R6" s="13" t="n">
         <f aca="false">INT(T6/U6)</f>
-        <v>119061</v>
+        <v>119180</v>
       </c>
       <c r="S6" s="14" t="n">
-        <v>2381226</v>
+        <v>2383600</v>
       </c>
       <c r="T6" s="13" t="n">
         <f aca="false">INT(S6/10)</f>
-        <v>238122</v>
+        <v>238360</v>
       </c>
       <c r="U6" s="11" t="n">
         <v>2</v>
@@ -897,14 +900,14 @@
       </c>
       <c r="R7" s="13" t="n">
         <f aca="false">INT(T7/U7)</f>
-        <v>237740</v>
+        <v>236874</v>
       </c>
       <c r="S7" s="14" t="n">
-        <v>4754819</v>
+        <v>4737490</v>
       </c>
       <c r="T7" s="13" t="n">
         <f aca="false">INT(S7/10)</f>
-        <v>475481</v>
+        <v>473749</v>
       </c>
       <c r="U7" s="11" t="n">
         <v>2</v>
@@ -962,14 +965,14 @@
       </c>
       <c r="R8" s="13" t="n">
         <f aca="false">INT(T8/U8)</f>
-        <v>212477</v>
+        <v>212537</v>
       </c>
       <c r="S8" s="14" t="n">
-        <v>4249541</v>
+        <v>4250745</v>
       </c>
       <c r="T8" s="13" t="n">
         <f aca="false">INT(S8/10)</f>
-        <v>424954</v>
+        <v>425074</v>
       </c>
       <c r="U8" s="11" t="n">
         <v>2</v>
@@ -1027,14 +1030,14 @@
       </c>
       <c r="R9" s="13" t="n">
         <f aca="false">INT(T9/U9)</f>
-        <v>282927</v>
+        <v>282926</v>
       </c>
       <c r="S9" s="14" t="n">
-        <v>5658556</v>
+        <v>5658527</v>
       </c>
       <c r="T9" s="13" t="n">
         <f aca="false">INT(S9/10)</f>
-        <v>565855</v>
+        <v>565852</v>
       </c>
       <c r="U9" s="11" t="n">
         <v>2</v>
@@ -1092,14 +1095,14 @@
       </c>
       <c r="R10" s="13" t="n">
         <f aca="false">INT(T10/U10)</f>
-        <v>538966</v>
+        <v>538383</v>
       </c>
       <c r="S10" s="14" t="n">
-        <v>10779339</v>
+        <v>10767679</v>
       </c>
       <c r="T10" s="13" t="n">
         <f aca="false">INT(S10/10)</f>
-        <v>1077933</v>
+        <v>1076767</v>
       </c>
       <c r="U10" s="11" t="n">
         <v>2</v>
@@ -1148,26 +1151,26 @@
       <c r="N11" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="O11" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P11" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="0" t="n">
-        <v>0</v>
+      <c r="O11" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P11" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q11" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R11" s="16" t="n">
         <f aca="false">INT(T11/U11)</f>
-        <v>237740</v>
+        <v>236874</v>
       </c>
       <c r="S11" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4754819</v>
+        <v>4737490</v>
       </c>
       <c r="T11" s="16" t="n">
         <f aca="false">INT(S11/10)</f>
-        <v>475481</v>
+        <v>473749</v>
       </c>
       <c r="U11" s="0" t="n">
         <v>2</v>
@@ -1218,26 +1221,26 @@
       <c r="N12" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="O12" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P12" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q12" s="0" t="n">
-        <v>0</v>
+      <c r="O12" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P12" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q12" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R12" s="16" t="n">
         <f aca="false">INT(T12/U12)</f>
-        <v>237740</v>
+        <v>236874</v>
       </c>
       <c r="S12" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4754819</v>
+        <v>4737490</v>
       </c>
       <c r="T12" s="16" t="n">
         <f aca="false">INT(S12/10)</f>
-        <v>475481</v>
+        <v>473749</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>2</v>
@@ -1290,26 +1293,26 @@
       <c r="N13" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="O13" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <v>4096</v>
+      <c r="O13" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P13" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q13" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R13" s="16" t="n">
         <f aca="false">INT(T13/U13)</f>
-        <v>1020</v>
+        <v>1325</v>
       </c>
       <c r="S13" s="0" t="n">
         <f aca="false">S$3</f>
-        <v>20403</v>
+        <v>26512</v>
       </c>
       <c r="T13" s="16" t="n">
         <f aca="false">INT(S13/10)</f>
-        <v>2040</v>
+        <v>2651</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>2</v>
@@ -1362,26 +1365,26 @@
       <c r="N14" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="O14" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q14" s="0" t="n">
-        <v>4096</v>
+      <c r="O14" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P14" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q14" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R14" s="16" t="n">
         <f aca="false">INT(T14/U14)</f>
-        <v>15679</v>
+        <v>15690</v>
       </c>
       <c r="S14" s="0" t="n">
         <f aca="false">S$4</f>
-        <v>313588</v>
+        <v>313813</v>
       </c>
       <c r="T14" s="16" t="n">
         <f aca="false">INT(S14/10)</f>
-        <v>31358</v>
+        <v>31381</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>2</v>
@@ -1434,26 +1437,26 @@
       <c r="N15" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="O15" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P15" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q15" s="0" t="n">
-        <v>4096</v>
+      <c r="O15" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P15" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q15" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R15" s="16" t="n">
         <f aca="false">INT(T15/U15)</f>
-        <v>83660</v>
+        <v>83701</v>
       </c>
       <c r="S15" s="0" t="n">
         <f aca="false">S$5</f>
-        <v>1673203</v>
+        <v>1674035</v>
       </c>
       <c r="T15" s="16" t="n">
         <f aca="false">INT(S15/10)</f>
-        <v>167320</v>
+        <v>167403</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>2</v>
@@ -1506,26 +1509,26 @@
       <c r="N16" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="O16" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P16" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q16" s="0" t="n">
-        <v>4096</v>
+      <c r="O16" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P16" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q16" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R16" s="16" t="n">
         <f aca="false">INT(T16/U16)</f>
-        <v>119061</v>
+        <v>119180</v>
       </c>
       <c r="S16" s="0" t="n">
         <f aca="false">S$6</f>
-        <v>2381226</v>
+        <v>2383600</v>
       </c>
       <c r="T16" s="16" t="n">
         <f aca="false">INT(S16/10)</f>
-        <v>238122</v>
+        <v>238360</v>
       </c>
       <c r="U16" s="0" t="n">
         <v>2</v>
@@ -1578,26 +1581,26 @@
       <c r="N17" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="O17" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P17" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q17" s="0" t="n">
-        <v>4096</v>
+      <c r="O17" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P17" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q17" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R17" s="16" t="n">
         <f aca="false">INT(T17/U17)</f>
-        <v>237740</v>
+        <v>236874</v>
       </c>
       <c r="S17" s="0" t="n">
         <f aca="false">S$7</f>
-        <v>4754819</v>
+        <v>4737490</v>
       </c>
       <c r="T17" s="16" t="n">
         <f aca="false">INT(S17/10)</f>
-        <v>475481</v>
+        <v>473749</v>
       </c>
       <c r="U17" s="0" t="n">
         <v>2</v>
@@ -1650,26 +1653,26 @@
       <c r="N18" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="O18" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P18" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q18" s="0" t="n">
-        <v>4096</v>
+      <c r="O18" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P18" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q18" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R18" s="16" t="n">
         <f aca="false">INT(T18/U18)</f>
-        <v>212477</v>
+        <v>212537</v>
       </c>
       <c r="S18" s="0" t="n">
         <f aca="false">S$8</f>
-        <v>4249541</v>
+        <v>4250745</v>
       </c>
       <c r="T18" s="16" t="n">
         <f aca="false">INT(S18/10)</f>
-        <v>424954</v>
+        <v>425074</v>
       </c>
       <c r="U18" s="0" t="n">
         <v>2</v>
@@ -1724,26 +1727,26 @@
       <c r="N19" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="O19" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P19" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q19" s="0" t="n">
-        <v>4096</v>
+      <c r="O19" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P19" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q19" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R19" s="16" t="n">
         <f aca="false">INT(T19/U19)</f>
-        <v>282927</v>
+        <v>282926</v>
       </c>
       <c r="S19" s="0" t="n">
         <f aca="false">S$9</f>
-        <v>5658556</v>
+        <v>5658527</v>
       </c>
       <c r="T19" s="16" t="n">
         <f aca="false">INT(S19/10)</f>
-        <v>565855</v>
+        <v>565852</v>
       </c>
       <c r="U19" s="0" t="n">
         <v>2</v>
@@ -1798,26 +1801,26 @@
       <c r="N20" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="O20" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="P20" s="0" t="n">
-        <v>4096</v>
-      </c>
-      <c r="Q20" s="0" t="n">
-        <v>4096</v>
+      <c r="O20" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="P20" s="1" t="n">
+        <v>1048576</v>
+      </c>
+      <c r="Q20" s="1" t="n">
+        <v>1048576</v>
       </c>
       <c r="R20" s="16" t="n">
         <f aca="false">INT(T20/U20)</f>
-        <v>538966</v>
+        <v>538383</v>
       </c>
       <c r="S20" s="0" t="n">
         <f aca="false">S$10</f>
-        <v>10779339</v>
+        <v>10767679</v>
       </c>
       <c r="T20" s="16" t="n">
         <f aca="false">INT(S20/10)</f>
-        <v>1077933</v>
+        <v>1076767</v>
       </c>
       <c r="U20" s="0" t="n">
         <v>2</v>
@@ -1826,18 +1829,68 @@
       <c r="W20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
-      <c r="B21" s="0"/>
-      <c r="C21" s="0"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="0" t="n">
+        <f aca="false">A20+1</f>
+        <v>19</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G21" s="15" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="0" t="s">
+        <v>54</v>
+      </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
+      <c r="N21" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="P21" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="Q21" s="1" t="n">
+        <v>2048</v>
+      </c>
+      <c r="R21" s="16" t="n">
+        <f aca="false">INT(T21/U21)/2</f>
+        <v>118437</v>
+      </c>
+      <c r="S21" s="0" t="n">
+        <f aca="false">S$7</f>
+        <v>4737490</v>
+      </c>
+      <c r="T21" s="16" t="n">
+        <f aca="false">INT(S21/10)</f>
+        <v>473749</v>
+      </c>
+      <c r="U21" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>

</xml_diff>